<commit_message>
Update Cleaning Summary with corrected version
</commit_message>
<xml_diff>
--- a/Docs/Cleaning_Summary.xlsx
+++ b/Docs/Cleaning_Summary.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ae3c32864a133e7/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{A36B98EA-8447-4003-8B3D-8D04681E05F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{360923BE-6713-4A7A-8BCF-2623CFF5353C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cleaning summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary statistics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Field</t>
   </si>
@@ -22,9 +29,6 @@
     <t>Cleaning Performed</t>
   </si>
   <si>
-    <t>Method Used / Description</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -49,59 +53,293 @@
     <t>All Fields</t>
   </si>
   <si>
-    <t>Removed duplicates</t>
-  </si>
-  <si>
-    <t>Removed prefixes, noisy suffixes, and fixed casing</t>
-  </si>
-  <si>
-    <t>Removed ages &gt; 65 and decimals</t>
-  </si>
-  <si>
     <t>Removed missing and invalid emails</t>
   </si>
   <si>
-    <t>Removed missing or invalid dates</t>
-  </si>
-  <si>
-    <t>Rounded decimals, removed unrealistic values</t>
-  </si>
-  <si>
-    <t>Fixed typos, replaced unexpected values with 'Unknown'</t>
-  </si>
-  <si>
     <t>Trimmed spaces, fixed casing</t>
   </si>
   <si>
     <t>drop_duplicates(subset='ID')</t>
   </si>
   <si>
-    <t>Used regex for mr/mrs, removed 'party', .title()</t>
-  </si>
-  <si>
-    <t>Filtered rows &gt; 65, converted to int using astype('int')</t>
-  </si>
-  <si>
-    <t>Validated using regex, removed NaNs and invalid format</t>
-  </si>
-  <si>
-    <t>Used pd.to_datetime() with errors='coerce', dropped NaT rows</t>
-  </si>
-  <si>
-    <t>Used round(), filtered values outside realistic salary range</t>
-  </si>
-  <si>
-    <t>Standardized casing, validated against known list</t>
-  </si>
-  <si>
-    <t>Applied str.strip() and str.title() where needed</t>
+    <t xml:space="preserve"> Description</t>
+  </si>
+  <si>
+    <t>Duplicate Removal</t>
+  </si>
+  <si>
+    <t>Removed duplicate IDs to ensure uniqueness</t>
+  </si>
+  <si>
+    <t>Transformation Applied</t>
+  </si>
+  <si>
+    <t>Assumption Made</t>
+  </si>
+  <si>
+    <t>ID must be unique for each row</t>
+  </si>
+  <si>
+    <t>Removed rows with missing values, trimmed extra spaces, removed prefixes (e.g., Mr, Mrs) from names, and standardized casing</t>
+  </si>
+  <si>
+    <r>
+      <t>Removed prefixes (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Mr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Mrs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">), 
+stripped suffixes like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>party</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.title()</t>
+    </r>
+  </si>
+  <si>
+    <t>Removed rows with age &gt; 65 and
+ decimal ages, converted to integer</t>
+  </si>
+  <si>
+    <t>Removed prefixes, noisy suffixes, null handling,
+and fixed casing</t>
+  </si>
+  <si>
+    <t>Null handling, data type conversion, outlier handling</t>
+  </si>
+  <si>
+    <t>Removed unrealistic age values (&lt;15 or &gt;65), missing values, and
+converted to integer</t>
+  </si>
+  <si>
+    <t>Validated format using regex; 
+dropped invalid or missing values</t>
+  </si>
+  <si>
+    <t>Only properly formatted email addresses are allowed</t>
+  </si>
+  <si>
+    <t>Age range assumed valid 
+between 15–65</t>
+  </si>
+  <si>
+    <t>Names should not include titles or extra descriptors</t>
+  </si>
+  <si>
+    <t>Null Handling, format validation</t>
+  </si>
+  <si>
+    <t>Dates must be valid and present</t>
+  </si>
+  <si>
+    <t>Null Handling, data type conversion, format validation</t>
+  </si>
+  <si>
+    <t>Removed missing or invalid dates,  converted to datetime format</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parsed using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>pd.to_datetime()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with errors='coerce', and
+dropped </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NaT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> values</t>
+    </r>
+  </si>
+  <si>
+    <t>Rounded decimal values, removed
+unrealistic outliers</t>
+  </si>
+  <si>
+    <t>Salaries expected to range from
+₹1,000 to ₹150,000</t>
+  </si>
+  <si>
+    <t>Removed missing values, converted to integers, removed salaries 
+outside ₹1,000 - ₹150,000 range</t>
+  </si>
+  <si>
+    <t>Standardized casing, removed 
+invalid entries</t>
+  </si>
+  <si>
+    <t>Only known department values
+ (Sales, HR, etc.) are accepted</t>
+  </si>
+  <si>
+    <t>Casing standardization, typo correction,
+unexpected value handling, null handling</t>
+  </si>
+  <si>
+    <t>Converted all values to title case, fixed common misspellings,
+ removed any value not in the valid list</t>
+  </si>
+  <si>
+    <t>Trimmed spaces, standardized text casing, dropped nulls in key fields, and ensured correct data types</t>
+  </si>
+  <si>
+    <t>All fields must be clean, consistently formatted, non-empty, and in their expected data types</t>
+  </si>
+  <si>
+    <t>Trimmed spaces, standardized casing, removed
+ nulls in key fields, and ensured correct data types</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Before Cleaning</t>
+  </si>
+  <si>
+    <t>After Cleaning</t>
+  </si>
+  <si>
+    <t>Total Rows</t>
+  </si>
+  <si>
+    <t>Duplicate IDs</t>
+  </si>
+  <si>
+    <t>Invalid Emails</t>
+  </si>
+  <si>
+    <t>Missing Age</t>
+  </si>
+  <si>
+    <t>Rows with Age &gt; 65</t>
+  </si>
+  <si>
+    <t>Missing Join Dates</t>
+  </si>
+  <si>
+    <t>Unrealistic Salaries</t>
+  </si>
+  <si>
+    <t>Name Prefixes Removed</t>
+  </si>
+  <si>
+    <t>Invalid Departments</t>
+  </si>
+  <si>
+    <t>~ 300</t>
+  </si>
+  <si>
+    <t>~3700</t>
+  </si>
+  <si>
+    <t>~1750</t>
+  </si>
+  <si>
+    <t>~1350</t>
+  </si>
+  <si>
+    <t>~2200</t>
+  </si>
+  <si>
+    <t>~1740</t>
+  </si>
+  <si>
+    <t>~2500</t>
+  </si>
+  <si>
+    <t>~1100</t>
+  </si>
+  <si>
+    <t>All cleaned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +355,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -153,24 +410,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +488,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -242,6 +522,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,9 +557,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,110 +733,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.1796875" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="25" customHeight="1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="46" customHeight="1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="58">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE531D9-15A1-4573-AF05-D731FE1EA556}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="26.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="6">
+        <v>11000</v>
+      </c>
+      <c r="C2">
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+        <v>62</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>